<commit_message>
subject todolist - hidden, register, delete, change
</commit_message>
<xml_diff>
--- a/Subject_Dir/ToDolist_Dir/SW테스트.xlsx
+++ b/Subject_Dir/ToDolist_Dir/SW테스트.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>과목</t>
   </si>
@@ -69,6 +69,39 @@
   </si>
   <si>
     <t>5월7일</t>
+  </si>
+  <si>
+    <t>테스트 케이스 설계 변경</t>
+  </si>
+  <si>
+    <t>7월19일</t>
+  </si>
+  <si>
+    <t>7월21일</t>
+  </si>
+  <si>
+    <t>준비</t>
+  </si>
+  <si>
+    <t>테스트 케이스 설계 수정</t>
+  </si>
+  <si>
+    <t>7월23일</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>테스트 케이스 수행</t>
+  </si>
+  <si>
+    <t>8월1일</t>
+  </si>
+  <si>
+    <t>8월2일</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>

</xml_diff>